<commit_message>
dataproperties and excel updates
</commit_message>
<xml_diff>
--- a/OpenemrMaven/src/test/resources/testdata/OpenEMRData.xlsx
+++ b/OpenemrMaven/src/test/resources/testdata/OpenEMRData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24321"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiDi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B-Mine\Company\Company\VFI-SLK\automation_workspace\OpenEmrApplication\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_D59A13312B723B71FC74E81F36350C5918C0C943" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="addPatientTest" sheetId="2" r:id="rId2"/>
+    <sheet name="checkHeaderAndVersionTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,46 +26,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>ExpectedValue</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Invalid username or password</t>
+  </si>
+  <si>
+    <t>peter123</t>
+  </si>
+  <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
   <si>
     <t>Username</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>ExpectedValue</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Invalid username or password</t>
-  </si>
-  <si>
-    <t>peter123</t>
-  </si>
-  <si>
-    <t>peter</t>
-  </si>
-  <si>
-    <t>Dutch</t>
+    <t>paul123</t>
+  </si>
+  <si>
+    <t>bala</t>
+  </si>
+  <si>
+    <t>bala123</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>1Invalid username or password2</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Dob</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>ExpectedAlertText</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>English (Indian)</t>
+  </si>
+  <si>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>dina</t>
+  </si>
+  <si>
+    <t>2021-07-20</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Tobacco</t>
+  </si>
+  <si>
+    <t>Medical Record Dashboard - Bala Dina</t>
+  </si>
+  <si>
+    <t>Expected Header</t>
+  </si>
+  <si>
+    <t>Expected Version Number</t>
+  </si>
+  <si>
+    <t>About OpenEMR</t>
+  </si>
+  <si>
+    <t>Version Number: v6.0.0 (1)</t>
+  </si>
+  <si>
+    <t>accountant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +163,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,60 +445,246 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>